<commit_message>
updated css and code to fix submit button issue
</commit_message>
<xml_diff>
--- a/FinalPresentation/GroupGrading.xlsx
+++ b/FinalPresentation/GroupGrading.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W0038182\OneDrive - Nova Scotia Community College\Classes\Winter2024\Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\5-Data Analytics Winter 2024\INFT3000 - Capstone\FinalPresentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE70290A-3E3D-4BEC-BD24-EE439AB089B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964A0609-CA16-4684-926B-2884B55DFD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grades" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Group Member</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Group Member Performance and Contribution</t>
   </si>
   <si>
-    <t>Effort and Commitment [Teamwork] (10pts)</t>
-  </si>
-  <si>
     <t>Teamwork (10pts)</t>
   </si>
   <si>
@@ -151,6 +148,39 @@
   </si>
   <si>
     <t>Skills and Knowedge (5pts)</t>
+  </si>
+  <si>
+    <t>James Laurence - w0211593</t>
+  </si>
+  <si>
+    <t>Gabriela Mkonde</t>
+  </si>
+  <si>
+    <t>Louise Fear</t>
+  </si>
+  <si>
+    <t>Chris Whalen</t>
+  </si>
+  <si>
+    <t>With Louise being sick for a few weeks, I was unable to rely on her for the tasks I delegated and had to increase my workload to compensate this.</t>
+  </si>
+  <si>
+    <t>Gabby, was always reliable to complete tasks within the timeframe, or provide reason as to why she couldn't.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chris did not show any initiative, had to wait to be told to do something. He seemed uninterested in doing anything outside his comfort zone of the material that was previously covered over the program. When I asked him to do something, he would try but would give up. (i.e. the xml extraction). With the minimum tasks that he did have, the time he spent on them was excessive, even though we were on a holding pattern due to the data extraction issue. he could have stepped up and offer to do other tasks, or even start something new. </t>
+  </si>
+  <si>
+    <t>Effort and Commitment 
+[Teamwork] (10pts)</t>
+  </si>
+  <si>
+    <t>Skills and 
+Knowedge (5pts)</t>
+  </si>
+  <si>
+    <t>Project Management
+and Coordination (5pts)</t>
   </si>
 </sst>
 </file>
@@ -251,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -282,6 +312,15 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,29 +605,32 @@
   <dimension ref="A2:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" customWidth="1"/>
-    <col min="4" max="4" width="46.42578125" customWidth="1"/>
-    <col min="5" max="5" width="63.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.33203125" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" s="14" t="s">
         <v>3</v>
       </c>
@@ -596,81 +638,120 @@
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="B6" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>8</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="1">
+        <f>SUM(B7:D7)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="1">
+        <f>SUM(B8:D8)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
         <v>2</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="1">
+        <f>SUM(B9:D9)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="17"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="12"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="12"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" s="12"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" s="12"/>
       <c r="D15" s="13"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" s="12"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="12"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="12"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="12"/>
     </row>
   </sheetData>
@@ -690,200 +771,200 @@
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="8.85546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="5.140625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="63.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.88671875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="5.109375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="63.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E2" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="5:12" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E4" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E5" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="5:12" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E6" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" s="7">
         <v>5</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="7">
         <v>5</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L6" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E7" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" s="7">
         <v>3</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I7" s="7">
         <v>3</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L7" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E8" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="7">
         <v>2</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" s="7">
         <v>2</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L8" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E9" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="7">
         <v>1</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I9" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E10" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="7">
         <v>0</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I10" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E12" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" s="3"/>
       <c r="K12" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="5:12" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E13" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" s="7">
         <v>5</v>
       </c>
       <c r="H13" s="3"/>
       <c r="K13" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L13" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E14" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" s="7">
         <v>3</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L14" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E15" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="7">
         <v>2</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L15" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E16" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F16" s="7">
         <v>1</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L16" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E17" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F17" s="7">
         <v>0</v>

</xml_diff>